<commit_message>
Created script to look for problems in the dataset
</commit_message>
<xml_diff>
--- a/Datasets/SeperateCountryFiles/Diamond_Princess.xlsx
+++ b/Datasets/SeperateCountryFiles/Diamond_Princess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gunsl_000\Desktop\COVID-19 By Country\COVID-19-By-Country\Datasets\SeperateCountryFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234047B0-8E05-4003-BC85-4715115456C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7262B2-7A37-4A27-B577-99AD40343815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="3675" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diamond_Princess" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -130,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1286,6 @@
         <v>691</v>
       </c>
       <c r="H20" s="1">
-        <f>G20-G19</f>
         <v>57</v>
       </c>
       <c r="I20" s="1">
@@ -1330,7 +1329,7 @@
         <v>691</v>
       </c>
       <c r="H21" s="1">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1">
         <v>3</v>

</xml_diff>